<commit_message>
changed the water decrease algorithm from the aphids so that it doesnt just double the decrease rate
</commit_message>
<xml_diff>
--- a/tools/flowerStats.xlsx
+++ b/tools/flowerStats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\github\ld46\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01107545-42D6-4F5B-AD9E-57C8AD57C54C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F43778-3CA4-4494-A794-7EEC2FBE08D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="1065" windowWidth="21600" windowHeight="11505" xr2:uid="{F9B10A4D-9A90-4E01-89B8-DD3631A5016B}"/>
+    <workbookView xWindow="13290" yWindow="1005" windowWidth="21600" windowHeight="11505" xr2:uid="{F9B10A4D-9A90-4E01-89B8-DD3631A5016B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +569,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
@@ -581,7 +581,7 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5">
         <f>B2/C2</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>

</xml_diff>

<commit_message>
Changed the flower arrangement and tweaks to watering rate
</commit_message>
<xml_diff>
--- a/tools/flowerStats.xlsx
+++ b/tools/flowerStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\github\ld46\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F43778-3CA4-4494-A794-7EEC2FBE08D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064FB3CD-733E-4781-A198-4F44DDD87CF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13290" yWindow="1005" windowWidth="21600" windowHeight="11505" xr2:uid="{F9B10A4D-9A90-4E01-89B8-DD3631A5016B}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +609,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="8">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D5" s="8">
         <v>5</v>
@@ -625,7 +625,7 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10">
         <f>B5/C5</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="10">
         <f>B5/D5</f>
@@ -659,7 +659,7 @@
         <v>175</v>
       </c>
       <c r="C8" s="2">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
@@ -675,7 +675,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5">
         <f>B8/C8</f>
-        <v>7</v>
+        <v>3.8888888888888888</v>
       </c>
       <c r="D9" s="5">
         <f>B8/D8</f>
@@ -709,7 +709,7 @@
         <v>150</v>
       </c>
       <c r="C11" s="8">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D11" s="8">
         <v>5</v>
@@ -725,7 +725,7 @@
       <c r="B12" s="10"/>
       <c r="C12" s="10">
         <f>B11/C11</f>
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="D12" s="10">
         <f>B11/D11</f>
@@ -759,7 +759,7 @@
         <v>100</v>
       </c>
       <c r="C14" s="2">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2">
         <v>4</v>
@@ -775,7 +775,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5">
         <f>B14/C14</f>
-        <v>6.666666666666667</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="D15" s="5">
         <f>B14/D14</f>
@@ -809,7 +809,7 @@
         <v>120</v>
       </c>
       <c r="C17" s="8">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D17" s="8">
         <v>5</v>
@@ -825,7 +825,7 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10">
         <f>B17/C17</f>
-        <v>10</v>
+        <v>3.4285714285714284</v>
       </c>
       <c r="D18" s="10">
         <f>B17/D17</f>
@@ -859,7 +859,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="2">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D20" s="2">
         <v>4</v>
@@ -875,7 +875,7 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5">
         <f>B20/C20</f>
-        <v>10</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="D21" s="5">
         <f>B20/D20</f>

</xml_diff>

<commit_message>
First initial balance run for levels 1-5
</commit_message>
<xml_diff>
--- a/tools/flowerStats.xlsx
+++ b/tools/flowerStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\github\ld46\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064FB3CD-733E-4781-A198-4F44DDD87CF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ECE500-3AE8-4584-9BCD-41B9DEF8DA14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13290" yWindow="1005" windowWidth="21600" windowHeight="11505" xr2:uid="{F9B10A4D-9A90-4E01-89B8-DD3631A5016B}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,10 +566,10 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C2" s="2">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
@@ -581,7 +581,7 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5">
         <f>B2/C2</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
@@ -609,7 +609,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D5" s="8">
         <v>5</v>
@@ -625,7 +625,7 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10">
         <f>B5/C5</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="10">
         <f>B5/D5</f>
@@ -659,7 +659,7 @@
         <v>175</v>
       </c>
       <c r="C8" s="2">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
@@ -675,7 +675,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5">
         <f>B8/C8</f>
-        <v>3.8888888888888888</v>
+        <v>1.9444444444444444</v>
       </c>
       <c r="D9" s="5">
         <f>B8/D8</f>
@@ -709,7 +709,7 @@
         <v>150</v>
       </c>
       <c r="C11" s="8">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D11" s="8">
         <v>5</v>
@@ -725,7 +725,7 @@
       <c r="B12" s="10"/>
       <c r="C12" s="10">
         <f>B11/C11</f>
-        <v>3.75</v>
+        <v>1.875</v>
       </c>
       <c r="D12" s="10">
         <f>B11/D11</f>
@@ -759,7 +759,7 @@
         <v>100</v>
       </c>
       <c r="C14" s="2">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2">
         <v>4</v>
@@ -775,7 +775,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5">
         <f>B14/C14</f>
-        <v>2.8571428571428572</v>
+        <v>1.4285714285714286</v>
       </c>
       <c r="D15" s="5">
         <f>B14/D14</f>
@@ -809,7 +809,7 @@
         <v>120</v>
       </c>
       <c r="C17" s="8">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D17" s="8">
         <v>5</v>
@@ -825,7 +825,7 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10">
         <f>B17/C17</f>
-        <v>3.4285714285714284</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="D18" s="10">
         <f>B17/D17</f>
@@ -859,7 +859,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D20" s="2">
         <v>4</v>
@@ -875,7 +875,7 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5">
         <f>B20/C20</f>
-        <v>2.6666666666666665</v>
+        <v>1.6</v>
       </c>
       <c r="D21" s="5">
         <f>B20/D20</f>

</xml_diff>